<commit_message>
Bug report start for Thong and a new test case
</commit_message>
<xml_diff>
--- a/Testing_Doc/BugReportTemplate.xlsx
+++ b/Testing_Doc/BugReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtran/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jere\Advanced Web Application Project\Testing_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C044CC7-AC03-B747-BA52-BFE23F0D37F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1367DCD3-B286-4CF0-87AB-5C0AE5F3A974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="500" windowWidth="33940" windowHeight="40980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case01" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>ID:</t>
   </si>
@@ -73,21 +73,9 @@
     <t>Priority:</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Steps to reproduce</t>
   </si>
   <si>
-    <t>Expected result</t>
-  </si>
-  <si>
-    <t>Actual result</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Jest encountered an unexpected token</t>
   </si>
   <si>
@@ -113,6 +101,30 @@
   </si>
   <si>
     <t>Actual result: Fail</t>
+  </si>
+  <si>
+    <t>Compiled with problems</t>
+  </si>
+  <si>
+    <t>29.11.2022</t>
+  </si>
+  <si>
+    <t>Description: Project failed to compile with errors</t>
+  </si>
+  <si>
+    <t>Expected result: Normal run of the project file with npm run dev</t>
+  </si>
+  <si>
+    <t>Actual result: Run error with missing modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steps to reproduce: npm run dev command </t>
+  </si>
+  <si>
+    <t>Thong Dang</t>
   </si>
 </sst>
 </file>
@@ -217,11 +229,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,6 +252,61 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>34229</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D0B0D40-3D18-D8CF-921C-0F08891A1436}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="333375" y="5848350"/>
+          <a:ext cx="7772400" cy="4472879"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -597,142 +664,150 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="82.33203125" customWidth="1"/>
+    <col min="3" max="3" width="82.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -744,6 +819,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -751,18 +827,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8573242-A2B4-A14F-B512-4D2B1DAF5479}">
   <dimension ref="B2:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="82.33203125" customWidth="1"/>
+    <col min="3" max="3" width="82.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,139 +846,139 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="3">
         <v>44886</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a test case and tried to fix a bug, didnt work yet
</commit_message>
<xml_diff>
--- a/Testing_Doc/BugReportTemplate.xlsx
+++ b/Testing_Doc/BugReportTemplate.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jere\Advanced Web Application Project\Testing_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1367DCD3-B286-4CF0-87AB-5C0AE5F3A974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1E1AF1-8AEC-4FC5-A57E-BD9BE7E1CB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case01" sheetId="1" r:id="rId1"/>
     <sheet name="Case02" sheetId="3" r:id="rId2"/>
+    <sheet name="Case03" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
   <si>
     <t>ID:</t>
   </si>
@@ -125,6 +126,18 @@
   </si>
   <si>
     <t>Thong Dang</t>
+  </si>
+  <si>
+    <t>Unexpected token Jest</t>
+  </si>
+  <si>
+    <t>Jere Muikku</t>
+  </si>
+  <si>
+    <t>Description : Automatic test failed to parse a file</t>
+  </si>
+  <si>
+    <t>Steps to reproduce: npm run test in Frontend</t>
   </si>
 </sst>
 </file>
@@ -388,6 +401,55 @@
         <a:xfrm>
           <a:off x="368299" y="20929600"/>
           <a:ext cx="15989231" cy="10033000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55175</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>75238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9695B626-7B08-8372-3B35-83B0187F66A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5905500"/>
+          <a:ext cx="15800000" cy="7695238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -664,7 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -828,7 +890,7 @@
   <dimension ref="B2:C108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,4 +1055,167 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B79381B-7BAF-400C-84B7-61E2670E3D85}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87.7109375" customWidth="1"/>
+    <col min="2" max="2" width="121" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44894</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="A27:B28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>